<commit_message>
Completed another 1600 dp problem
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D7AE5C-A9C8-487B-B20A-FED8B432AAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2441A68B-EB96-482C-9D76-5AC7B6CD9305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2388" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Prefix sums" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="501">
   <si>
     <t>Date</t>
   </si>
@@ -1517,6 +1518,18 @@
   </si>
   <si>
     <t>Just a classic 3d dp : Not 4d you fool! This is because both the robots will stay on the same row.</t>
+  </si>
+  <si>
+    <t>Sky Stars</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Prefix sums</t>
+  </si>
+  <si>
+    <t>The key is to see that c only has 11 possible values so we can store how many coordinates have a particular value of c . This can be done using a 11 X 101 X 101 3D vector.</t>
   </si>
 </sst>
 </file>
@@ -1887,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D192" zoomScale="92" workbookViewId="0">
+    <sheetView topLeftCell="D192" zoomScale="92" workbookViewId="0">
       <selection activeCell="F201" sqref="F201"/>
     </sheetView>
   </sheetViews>
@@ -5735,7 +5748,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5788,4 +5801,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1981E339-2796-4976-A33C-4CD16AAFE2F6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>499</v>
+      </c>
+      <c r="E2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E840AA7C-F337-41F0-9A9F-73979F88D83B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: solved the Halloween array problem of starters 164
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2441A68B-EB96-482C-9D76-5AC7B6CD9305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4136A2-3B0B-4E1E-9A66-35D60018B55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="503">
   <si>
     <t>Date</t>
   </si>
@@ -1530,6 +1530,12 @@
   </si>
   <si>
     <t>The key is to see that c only has 11 possible values so we can store how many coordinates have a particular value of c . This can be done using a 11 X 101 X 101 3D vector.</t>
+  </si>
+  <si>
+    <t>Halloween Array</t>
+  </si>
+  <si>
+    <t>The first thing to notice is the fact that if even one number is repeated then f(A)=0 and we can check the rest. If no element is repeated then if n&gt;32 then as r&lt;=1e9 the value of f(A) &gt; 1e9 and theus f(A)&gt;r . And for n&lt;=32 brute force.</t>
   </si>
 </sst>
 </file>
@@ -1898,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView topLeftCell="D192" zoomScale="92" workbookViewId="0">
-      <selection activeCell="F201" sqref="F201"/>
+    <sheetView tabSelected="1" topLeftCell="C179" zoomScale="92" workbookViewId="0">
+      <selection activeCell="F202" sqref="F202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5645,6 +5651,23 @@
       </c>
       <c r="F200" t="s">
         <v>496</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B201" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C201" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" t="s">
+        <v>435</v>
+      </c>
+      <c r="F201" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -5738,6 +5761,7 @@
     <hyperlink ref="B184" r:id="rId86" xr:uid="{6C4D878D-9002-40C0-BF89-99F9B5027E75}"/>
     <hyperlink ref="B183" r:id="rId87" xr:uid="{3D5294C5-755E-4029-B98F-7321D2C91F6C}"/>
     <hyperlink ref="B182" r:id="rId88" xr:uid="{5C08971A-F22C-4825-A7D0-882AFF3AB137}"/>
+    <hyperlink ref="B201" r:id="rId89" xr:uid="{397CE38A-C841-4E1E-B379-4BF7C48F5816}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5807,7 +5831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1981E339-2796-4976-A33C-4CD16AAFE2F6}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: implement prim's algorithm, DSU and krushkal's algorithm
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4136A2-3B0B-4E1E-9A66-35D60018B55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFEF161-713D-4E2D-B3C2-C555E7133C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="511">
   <si>
     <t>Date</t>
   </si>
@@ -1536,6 +1536,30 @@
   </si>
   <si>
     <t>The first thing to notice is the fact that if even one number is repeated then f(A)=0 and we can check the rest. If no element is repeated then if n&gt;32 then as r&lt;=1e9 the value of f(A) &gt; 1e9 and theus f(A)&gt;r . And for n&lt;=32 brute force.</t>
+  </si>
+  <si>
+    <t>Mishkin Energizer</t>
+  </si>
+  <si>
+    <t>String + implementation</t>
+  </si>
+  <si>
+    <t>Its very hard to explain this , the only thing I learnt from this is that I need to try harder in problems(doesn't mean give more time,  it means think more clearly)</t>
+  </si>
+  <si>
+    <t>Path With Minimum Effort</t>
+  </si>
+  <si>
+    <t>You use bfs but greedily , for each node in the current queue we choose the one which has currently lowest effort and thus we need a priority queue.</t>
+  </si>
+  <si>
+    <t>Find Minimum Time to Reach Last Room II</t>
+  </si>
+  <si>
+    <t>Shortest path</t>
+  </si>
+  <si>
+    <t>This pattern is very useful the bfs modified with the priority queue or set, however here set works but pq gives tle</t>
   </si>
 </sst>
 </file>
@@ -1904,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C179" zoomScale="92" workbookViewId="0">
-      <selection activeCell="F202" sqref="F202"/>
+    <sheetView tabSelected="1" topLeftCell="C186" zoomScale="92" workbookViewId="0">
+      <selection activeCell="F205" sqref="F205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5637,7 +5661,7 @@
       <c r="A200" t="s">
         <v>303</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="1" t="s">
         <v>495</v>
       </c>
       <c r="C200" t="s">
@@ -5668,6 +5692,57 @@
       </c>
       <c r="F201" t="s">
         <v>502</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B202" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C202" t="s">
+        <v>6</v>
+      </c>
+      <c r="D202" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" t="s">
+        <v>504</v>
+      </c>
+      <c r="F202" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B203" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C203" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" t="s">
+        <v>509</v>
+      </c>
+      <c r="F203" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B204" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C204" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" t="s">
+        <v>6</v>
+      </c>
+      <c r="E204" t="s">
+        <v>509</v>
+      </c>
+      <c r="F204" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -5762,6 +5837,10 @@
     <hyperlink ref="B183" r:id="rId87" xr:uid="{3D5294C5-755E-4029-B98F-7321D2C91F6C}"/>
     <hyperlink ref="B182" r:id="rId88" xr:uid="{5C08971A-F22C-4825-A7D0-882AFF3AB137}"/>
     <hyperlink ref="B201" r:id="rId89" xr:uid="{397CE38A-C841-4E1E-B379-4BF7C48F5816}"/>
+    <hyperlink ref="B202" r:id="rId90" xr:uid="{849E95C3-FEE5-4AA5-90F9-1FB6AFB5D077}"/>
+    <hyperlink ref="B203" r:id="rId91" xr:uid="{C578028F-497B-43F4-B0E4-CCB3BBBBDBC9}"/>
+    <hyperlink ref="B200" r:id="rId92" xr:uid="{E081DD8D-8959-43DB-8338-3ADCF7FB1676}"/>
+    <hyperlink ref="B204" r:id="rId93" xr:uid="{D22A4362-2F9D-48ED-85DC-57B875849283}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: implement kosaraju's algorithm
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFEF161-713D-4E2D-B3C2-C555E7133C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F266EB9-3B38-44EE-B19F-80C3B0F4925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="513">
   <si>
     <t>Date</t>
   </si>
@@ -1560,6 +1560,12 @@
   </si>
   <si>
     <t>This pattern is very useful the bfs modified with the priority queue or set, however here set works but pq gives tle</t>
+  </si>
+  <si>
+    <t>Permutation Game</t>
+  </si>
+  <si>
+    <t>your dp skills need work.</t>
   </si>
 </sst>
 </file>
@@ -1928,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:F205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C186" zoomScale="92" workbookViewId="0">
-      <selection activeCell="F205" sqref="F205"/>
+    <sheetView tabSelected="1" topLeftCell="C184" zoomScale="92" workbookViewId="0">
+      <selection activeCell="F206" sqref="F206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5743,6 +5749,23 @@
       </c>
       <c r="F204" t="s">
         <v>510</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B205" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C205" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205" t="s">
+        <v>7</v>
+      </c>
+      <c r="E205" t="s">
+        <v>333</v>
+      </c>
+      <c r="F205" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -5841,6 +5864,7 @@
     <hyperlink ref="B203" r:id="rId91" xr:uid="{C578028F-497B-43F4-B0E4-CCB3BBBBDBC9}"/>
     <hyperlink ref="B200" r:id="rId92" xr:uid="{E081DD8D-8959-43DB-8338-3ADCF7FB1676}"/>
     <hyperlink ref="B204" r:id="rId93" xr:uid="{D22A4362-2F9D-48ED-85DC-57B875849283}"/>
+    <hyperlink ref="B205" r:id="rId94" xr:uid="{F71F6C23-95B8-4F97-91E2-1FD123B66BE1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat : implement the seive of eratosthenes
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F266EB9-3B38-44EE-B19F-80C3B0F4925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F79AB7A-DF38-4593-B050-2C03B75D3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="515">
   <si>
     <t>Date</t>
   </si>
@@ -1566,6 +1566,12 @@
   </si>
   <si>
     <t>your dp skills need work.</t>
+  </si>
+  <si>
+    <t>Number of greater elements to the right</t>
+  </si>
+  <si>
+    <t>when you think that you need to check for all pairs (I,j) for an array it is important to consider the count inversions way.</t>
   </si>
 </sst>
 </file>
@@ -1934,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
-  <dimension ref="A1:F205"/>
+  <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C184" zoomScale="92" workbookViewId="0">
-      <selection activeCell="F206" sqref="F206"/>
+    <sheetView tabSelected="1" topLeftCell="C195" zoomScale="92" workbookViewId="0">
+      <selection activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5766,6 +5772,23 @@
       </c>
       <c r="F205" t="s">
         <v>512</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B206" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C206" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206" t="s">
+        <v>7</v>
+      </c>
+      <c r="E206" t="s">
+        <v>301</v>
+      </c>
+      <c r="F206" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -5865,6 +5888,7 @@
     <hyperlink ref="B200" r:id="rId92" xr:uid="{E081DD8D-8959-43DB-8338-3ADCF7FB1676}"/>
     <hyperlink ref="B204" r:id="rId93" xr:uid="{D22A4362-2F9D-48ED-85DC-57B875849283}"/>
     <hyperlink ref="B205" r:id="rId94" xr:uid="{F71F6C23-95B8-4F97-91E2-1FD123B66BE1}"/>
+    <hyperlink ref="B206" r:id="rId95" xr:uid="{80705264-AD97-44FE-AC3C-47F56E15F4FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Solve the problem breach of faith
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F79AB7A-DF38-4593-B050-2C03B75D3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC5B9A-2785-402C-9961-A3A409F83173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="527">
   <si>
     <t>Date</t>
   </si>
@@ -1572,6 +1572,42 @@
   </si>
   <si>
     <t>when you think that you need to check for all pairs (I,j) for an array it is important to consider the count inversions way.</t>
+  </si>
+  <si>
+    <t>Combination Sum 2</t>
+  </si>
+  <si>
+    <t>I have realized that the most important aspect of backtracking is pruning of the tree.</t>
+  </si>
+  <si>
+    <t>Preorder, Postorder and Inorder Traversal of a Binary Tree using a single Stack</t>
+  </si>
+  <si>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>Partition Array Into Two Arrays to Minimize Sum Difference</t>
+  </si>
+  <si>
+    <t>Meet in the middle</t>
+  </si>
+  <si>
+    <t>Print Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>dp on LIS</t>
+  </si>
+  <si>
+    <t>try in O(nlogn)</t>
+  </si>
+  <si>
+    <t>Gas station</t>
+  </si>
+  <si>
+    <t>repititive</t>
+  </si>
+  <si>
+    <t>Count Partitions With Max-Min Difference at Most K</t>
   </si>
 </sst>
 </file>
@@ -1940,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
-  <dimension ref="A1:F206"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C195" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E207" sqref="E207"/>
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="92" workbookViewId="0">
+      <selection activeCell="E213" sqref="E213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5789,6 +5825,102 @@
       </c>
       <c r="F206" t="s">
         <v>514</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B207" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" t="s">
+        <v>418</v>
+      </c>
+      <c r="F207" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B208" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C208" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" t="s">
+        <v>7</v>
+      </c>
+      <c r="E208" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B209" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C209" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209" t="s">
+        <v>7</v>
+      </c>
+      <c r="E209" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>303</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C210" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" t="s">
+        <v>7</v>
+      </c>
+      <c r="E210" t="s">
+        <v>522</v>
+      </c>
+      <c r="F210" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>525</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C211" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" t="s">
+        <v>7</v>
+      </c>
+      <c r="E211" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B212" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C212" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" t="s">
+        <v>7</v>
+      </c>
+      <c r="E212" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5889,6 +6021,12 @@
     <hyperlink ref="B204" r:id="rId93" xr:uid="{D22A4362-2F9D-48ED-85DC-57B875849283}"/>
     <hyperlink ref="B205" r:id="rId94" xr:uid="{F71F6C23-95B8-4F97-91E2-1FD123B66BE1}"/>
     <hyperlink ref="B206" r:id="rId95" xr:uid="{80705264-AD97-44FE-AC3C-47F56E15F4FD}"/>
+    <hyperlink ref="B207" r:id="rId96" xr:uid="{A7FBEB65-87C6-4596-87F7-F5E968ACFCA2}"/>
+    <hyperlink ref="B208" r:id="rId97" xr:uid="{3A0EFFEA-5602-48F3-A883-C701BD7665F0}"/>
+    <hyperlink ref="B209" r:id="rId98" xr:uid="{C3C6DA5B-638B-4F34-8C47-D00EC6D0A86F}"/>
+    <hyperlink ref="B210" r:id="rId99" xr:uid="{CF95A913-4896-45EF-87ED-11671A6B734E}"/>
+    <hyperlink ref="B211" r:id="rId100" xr:uid="{11984A4C-4DC9-4759-AC42-E1B8A4FD3B0B}"/>
+    <hyperlink ref="B212" r:id="rId101" xr:uid="{E1C92969-3912-46AE-9CA2-D935FA7D2A88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Solved today's leetcode POTD
</commit_message>
<xml_diff>
--- a/Marked questions.xlsx
+++ b/Marked questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amrutanshu\Desktop\codefiles\CP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDC5B9A-2785-402C-9961-A3A409F83173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65264724-782D-4401-971D-B7A700220B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44586737-5555-46D0-B19C-B395521DBDB7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="528">
   <si>
     <t>Date</t>
   </si>
@@ -1608,6 +1608,9 @@
   </si>
   <si>
     <t>Count Partitions With Max-Min Difference at Most K</t>
+  </si>
+  <si>
+    <t>Maximize Subarrays After Removing One Conflicting Pair</t>
   </si>
 </sst>
 </file>
@@ -1976,10 +1979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47F879-41D9-4209-8775-ED012ABB8653}">
-  <dimension ref="A1:F212"/>
+  <dimension ref="A1:F213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E213" sqref="E213"/>
+    <sheetView tabSelected="1" topLeftCell="C198" zoomScale="92" workbookViewId="0">
+      <selection activeCell="F214" sqref="F214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5921,6 +5924,23 @@
       </c>
       <c r="E212" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B213" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C213" t="s">
+        <v>7</v>
+      </c>
+      <c r="D213" t="s">
+        <v>7</v>
+      </c>
+      <c r="E213" t="s">
+        <v>333</v>
+      </c>
+      <c r="F213" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -6027,6 +6047,7 @@
     <hyperlink ref="B210" r:id="rId99" xr:uid="{CF95A913-4896-45EF-87ED-11671A6B734E}"/>
     <hyperlink ref="B211" r:id="rId100" xr:uid="{11984A4C-4DC9-4759-AC42-E1B8A4FD3B0B}"/>
     <hyperlink ref="B212" r:id="rId101" xr:uid="{E1C92969-3912-46AE-9CA2-D935FA7D2A88}"/>
+    <hyperlink ref="B213" r:id="rId102" xr:uid="{E8FF6A36-8F2D-4635-BFFE-2E378DA53587}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>